<commit_message>
the last version 12 dec
</commit_message>
<xml_diff>
--- a/AI_yes_no.xlsx
+++ b/AI_yes_no.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>https://rabota.ua/cv/5669965</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>link</t>
+  </si>
+  <si>
+    <t>https://rabota.ua/cv/3787170</t>
   </si>
 </sst>
 </file>
@@ -490,9 +493,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A41"/>
+  <dimension ref="A1:A42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -559,149 +564,154 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>